<commit_message>
excel read file anme
</commit_message>
<xml_diff>
--- a/items.xlsx
+++ b/items.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\곰치\Desktop\TFI\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A37E3602-DC94-480F-BA1A-0F4ADB8D2171}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2781EBA-A282-4833-9E1D-3A10A6CC8DC2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{5E2D2B26-9E3D-45A7-9237-86961CAF8455}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="150">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="151">
   <si>
     <t>laptop</t>
   </si>
@@ -1262,6 +1262,10 @@
   </si>
   <si>
     <t>해롭다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>음..</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1673,7 +1677,7 @@
   <dimension ref="A1:E75"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -1725,6 +1729,9 @@
       <c r="D3" s="1">
         <v>1</v>
       </c>
+      <c r="E3" t="s">
+        <v>150</v>
+      </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">

</xml_diff>

<commit_message>
data read error handle
</commit_message>
<xml_diff>
--- a/items.xlsx
+++ b/items.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\곰치\Desktop\TFI\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2781EBA-A282-4833-9E1D-3A10A6CC8DC2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23D2ED62-499F-4B70-8254-8EE4D2E7D8A6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{5E2D2B26-9E3D-45A7-9237-86961CAF8455}"/>
+    <workbookView xWindow="12315" yWindow="3075" windowWidth="21600" windowHeight="11385" xr2:uid="{5E2D2B26-9E3D-45A7-9237-86961CAF8455}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1231,41 +1231,31 @@
     </r>
   </si>
   <si>
-    <t>volume(100ml)</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>weight(100g)</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>Name</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="맑은 고딕"/>
-        <family val="3"/>
-        <charset val="129"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>이름</t>
-    </r>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>상세정보</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>해롭다.</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>음..</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>korName</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>name</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>weight</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>volume</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>description</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1334,12 +1324,13 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="표준" xfId="0" builtinId="0"/>
@@ -1677,26 +1668,26 @@
   <dimension ref="A1:E75"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
+        <v>146</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>147</v>
       </c>
-      <c r="B1" s="2" t="s">
-        <v>146</v>
-      </c>
       <c r="C1" s="2" t="s">
-        <v>145</v>
+        <v>148</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>144</v>
+        <v>149</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>148</v>
+        <v>150</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
@@ -1713,7 +1704,7 @@
         <v>1</v>
       </c>
       <c r="E2" t="s">
-        <v>149</v>
+        <v>144</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
@@ -1730,7 +1721,7 @@
         <v>1</v>
       </c>
       <c r="E3" t="s">
-        <v>150</v>
+        <v>145</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">

</xml_diff>